<commit_message>
add timesheet; fix incorection in the S0; add data from first annotator
</commit_message>
<xml_diff>
--- a/experiments/human-evaluation/01-experimental-sample/S0-excel.xlsx
+++ b/experiments/human-evaluation/01-experimental-sample/S0-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-works\github\uder-annotation-interface\experiments\human-evaluation\01-experimental-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB39AA4-4B20-42E7-A2E6-4030FE38158F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3675BA-6042-4427-A27E-488330EBFD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="268">
   <si>
     <t>+</t>
   </si>
@@ -1682,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C375"/>
+  <dimension ref="A1:C374"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="G359" sqref="G359"/>
+    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
+      <selection activeCell="E247" sqref="E247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,7 +4184,7 @@
         <v>175</v>
       </c>
       <c r="C240" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -4192,10 +4192,10 @@
         <v>0</v>
       </c>
       <c r="B241" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C241" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -4203,10 +4203,10 @@
         <v>0</v>
       </c>
       <c r="B242" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C242" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -4217,7 +4217,7 @@
         <v>180</v>
       </c>
       <c r="C243" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -4228,7 +4228,7 @@
         <v>180</v>
       </c>
       <c r="C244" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -4236,10 +4236,10 @@
         <v>0</v>
       </c>
       <c r="B245" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C245" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -4250,7 +4250,7 @@
         <v>178</v>
       </c>
       <c r="C246" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v>178</v>
       </c>
       <c r="C247" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -4272,7 +4272,7 @@
         <v>178</v>
       </c>
       <c r="C248" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -4283,7 +4283,7 @@
         <v>178</v>
       </c>
       <c r="C249" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -4291,10 +4291,10 @@
         <v>0</v>
       </c>
       <c r="B250" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C250" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -4305,7 +4305,7 @@
         <v>179</v>
       </c>
       <c r="C251" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -4316,7 +4316,7 @@
         <v>179</v>
       </c>
       <c r="C252" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -4324,10 +4324,10 @@
         <v>0</v>
       </c>
       <c r="B253" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C253" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -4335,10 +4335,10 @@
         <v>0</v>
       </c>
       <c r="B254" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C254" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -4349,7 +4349,7 @@
         <v>177</v>
       </c>
       <c r="C255" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -4360,18 +4360,18 @@
         <v>177</v>
       </c>
       <c r="C256" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>0</v>
-      </c>
-      <c r="B257" t="s">
-        <v>177</v>
-      </c>
-      <c r="C257" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>0</v>
+      </c>
+      <c r="B258" t="s">
+        <v>193</v>
+      </c>
+      <c r="C258" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -4382,7 +4382,7 @@
         <v>193</v>
       </c>
       <c r="C259" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -4393,7 +4393,7 @@
         <v>193</v>
       </c>
       <c r="C260" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -4404,7 +4404,7 @@
         <v>193</v>
       </c>
       <c r="C261" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -4415,7 +4415,7 @@
         <v>193</v>
       </c>
       <c r="C262" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -4426,7 +4426,7 @@
         <v>193</v>
       </c>
       <c r="C263" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -4437,7 +4437,7 @@
         <v>193</v>
       </c>
       <c r="C264" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -4445,10 +4445,10 @@
         <v>0</v>
       </c>
       <c r="B265" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C265" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -4459,7 +4459,7 @@
         <v>195</v>
       </c>
       <c r="C266" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
         <v>195</v>
       </c>
       <c r="C267" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -4478,10 +4478,10 @@
         <v>0</v>
       </c>
       <c r="B268" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C268" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -4492,7 +4492,7 @@
         <v>201</v>
       </c>
       <c r="C269" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -4500,10 +4500,10 @@
         <v>0</v>
       </c>
       <c r="B270" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C270" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -4514,7 +4514,7 @@
         <v>197</v>
       </c>
       <c r="C271" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -4525,7 +4525,7 @@
         <v>197</v>
       </c>
       <c r="C272" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -4533,10 +4533,10 @@
         <v>0</v>
       </c>
       <c r="B273" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C273" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -4547,7 +4547,7 @@
         <v>194</v>
       </c>
       <c r="C274" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -4558,7 +4558,7 @@
         <v>194</v>
       </c>
       <c r="C275" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -4569,7 +4569,7 @@
         <v>194</v>
       </c>
       <c r="C276" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -4577,7 +4577,7 @@
         <v>0</v>
       </c>
       <c r="B277" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C277" t="s">
         <v>208</v>
@@ -4591,7 +4591,7 @@
         <v>205</v>
       </c>
       <c r="C278" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -4602,7 +4602,7 @@
         <v>205</v>
       </c>
       <c r="C279" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -4610,10 +4610,10 @@
         <v>0</v>
       </c>
       <c r="B280" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C280" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -4624,18 +4624,18 @@
         <v>196</v>
       </c>
       <c r="C281" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>0</v>
-      </c>
-      <c r="B282" t="s">
-        <v>196</v>
-      </c>
-      <c r="C282" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>0</v>
+      </c>
+      <c r="B283" t="s">
+        <v>212</v>
+      </c>
+      <c r="C283" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -4646,7 +4646,7 @@
         <v>212</v>
       </c>
       <c r="C284" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -4657,7 +4657,7 @@
         <v>212</v>
       </c>
       <c r="C285" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -4665,10 +4665,10 @@
         <v>0</v>
       </c>
       <c r="B286" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C286" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -4679,7 +4679,7 @@
         <v>216</v>
       </c>
       <c r="C287" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -4687,10 +4687,10 @@
         <v>0</v>
       </c>
       <c r="B288" t="s">
+        <v>217</v>
+      </c>
+      <c r="C288" t="s">
         <v>216</v>
-      </c>
-      <c r="C288" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -4698,10 +4698,10 @@
         <v>0</v>
       </c>
       <c r="B289" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C289" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -4712,7 +4712,7 @@
         <v>219</v>
       </c>
       <c r="C290" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -4723,7 +4723,7 @@
         <v>219</v>
       </c>
       <c r="C291" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -4734,7 +4734,7 @@
         <v>219</v>
       </c>
       <c r="C292" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -4745,7 +4745,7 @@
         <v>219</v>
       </c>
       <c r="C293" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -4753,10 +4753,10 @@
         <v>0</v>
       </c>
       <c r="B294" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C294" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -4767,7 +4767,7 @@
         <v>220</v>
       </c>
       <c r="C295" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -4778,7 +4778,7 @@
         <v>220</v>
       </c>
       <c r="C296" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -4786,10 +4786,10 @@
         <v>0</v>
       </c>
       <c r="B297" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C297" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -4797,10 +4797,10 @@
         <v>0</v>
       </c>
       <c r="B298" t="s">
+        <v>224</v>
+      </c>
+      <c r="C298" t="s">
         <v>223</v>
-      </c>
-      <c r="C298" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -4808,10 +4808,10 @@
         <v>0</v>
       </c>
       <c r="B299" t="s">
+        <v>218</v>
+      </c>
+      <c r="C299" t="s">
         <v>224</v>
-      </c>
-      <c r="C299" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -4822,18 +4822,18 @@
         <v>218</v>
       </c>
       <c r="C300" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>0</v>
-      </c>
-      <c r="B301" t="s">
-        <v>218</v>
-      </c>
-      <c r="C301" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>0</v>
+      </c>
+      <c r="B302" t="s">
+        <v>226</v>
+      </c>
+      <c r="C302" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -4841,10 +4841,10 @@
         <v>0</v>
       </c>
       <c r="B303" t="s">
+        <v>228</v>
+      </c>
+      <c r="C303" t="s">
         <v>226</v>
-      </c>
-      <c r="C303" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -4855,7 +4855,7 @@
         <v>228</v>
       </c>
       <c r="C304" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>228</v>
       </c>
       <c r="C305" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -4874,7 +4874,7 @@
         <v>0</v>
       </c>
       <c r="B306" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C306" t="s">
         <v>230</v>
@@ -4888,7 +4888,7 @@
         <v>229</v>
       </c>
       <c r="C307" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -4896,10 +4896,10 @@
         <v>0</v>
       </c>
       <c r="B308" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C308" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -4907,10 +4907,10 @@
         <v>0</v>
       </c>
       <c r="B309" t="s">
+        <v>230</v>
+      </c>
+      <c r="C309" t="s">
         <v>231</v>
-      </c>
-      <c r="C309" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -4918,10 +4918,10 @@
         <v>0</v>
       </c>
       <c r="B310" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C310" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -4932,7 +4932,7 @@
         <v>233</v>
       </c>
       <c r="C311" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -4943,7 +4943,7 @@
         <v>233</v>
       </c>
       <c r="C312" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -4954,7 +4954,7 @@
         <v>233</v>
       </c>
       <c r="C313" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -4965,7 +4965,7 @@
         <v>233</v>
       </c>
       <c r="C314" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -4973,21 +4973,21 @@
         <v>0</v>
       </c>
       <c r="B315" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C315" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
-        <v>0</v>
-      </c>
-      <c r="B316" t="s">
-        <v>235</v>
-      </c>
-      <c r="C316" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>0</v>
+      </c>
+      <c r="B317" t="s">
+        <v>237</v>
+      </c>
+      <c r="C317" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -4995,10 +4995,10 @@
         <v>0</v>
       </c>
       <c r="B318" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C318" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -5009,7 +5009,7 @@
         <v>239</v>
       </c>
       <c r="C319" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -5020,7 +5020,7 @@
         <v>239</v>
       </c>
       <c r="C320" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -5028,10 +5028,10 @@
         <v>0</v>
       </c>
       <c r="B321" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C321" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -5042,7 +5042,7 @@
         <v>241</v>
       </c>
       <c r="C322" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -5053,7 +5053,7 @@
         <v>241</v>
       </c>
       <c r="C323" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -5064,7 +5064,7 @@
         <v>241</v>
       </c>
       <c r="C324" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -5075,7 +5075,7 @@
         <v>241</v>
       </c>
       <c r="C325" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -5083,10 +5083,10 @@
         <v>0</v>
       </c>
       <c r="B326" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C326" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -5094,10 +5094,10 @@
         <v>0</v>
       </c>
       <c r="B327" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C327" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -5108,7 +5108,7 @@
         <v>243</v>
       </c>
       <c r="C328" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -5119,7 +5119,7 @@
         <v>243</v>
       </c>
       <c r="C329" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -5130,7 +5130,7 @@
         <v>243</v>
       </c>
       <c r="C330" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -5138,10 +5138,10 @@
         <v>0</v>
       </c>
       <c r="B331" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C331" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
@@ -5152,7 +5152,7 @@
         <v>248</v>
       </c>
       <c r="C332" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
@@ -5160,10 +5160,10 @@
         <v>0</v>
       </c>
       <c r="B333" t="s">
+        <v>247</v>
+      </c>
+      <c r="C333" t="s">
         <v>248</v>
-      </c>
-      <c r="C333" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
@@ -5171,10 +5171,10 @@
         <v>0</v>
       </c>
       <c r="B334" t="s">
+        <v>244</v>
+      </c>
+      <c r="C334" t="s">
         <v>247</v>
-      </c>
-      <c r="C334" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -5182,10 +5182,10 @@
         <v>0</v>
       </c>
       <c r="B335" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="C335" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>250</v>
       </c>
       <c r="C336" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
@@ -5204,10 +5204,10 @@
         <v>0</v>
       </c>
       <c r="B337" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C337" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
@@ -5218,7 +5218,7 @@
         <v>246</v>
       </c>
       <c r="C338" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -5229,7 +5229,7 @@
         <v>246</v>
       </c>
       <c r="C339" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -5240,18 +5240,18 @@
         <v>246</v>
       </c>
       <c r="C340" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
-        <v>0</v>
-      </c>
-      <c r="B341" t="s">
-        <v>246</v>
-      </c>
-      <c r="C341" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>0</v>
+      </c>
+      <c r="B342" t="s">
+        <v>255</v>
+      </c>
+      <c r="C342" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -5262,7 +5262,7 @@
         <v>255</v>
       </c>
       <c r="C343" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
@@ -5273,7 +5273,7 @@
         <v>255</v>
       </c>
       <c r="C344" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
@@ -5284,7 +5284,7 @@
         <v>255</v>
       </c>
       <c r="C345" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -5292,10 +5292,10 @@
         <v>0</v>
       </c>
       <c r="B346" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C346" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -5306,7 +5306,7 @@
         <v>256</v>
       </c>
       <c r="C347" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -5317,7 +5317,7 @@
         <v>256</v>
       </c>
       <c r="C348" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -5328,7 +5328,7 @@
         <v>256</v>
       </c>
       <c r="C349" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
@@ -5336,10 +5336,10 @@
         <v>0</v>
       </c>
       <c r="B350" t="s">
+        <v>258</v>
+      </c>
+      <c r="C350" t="s">
         <v>256</v>
-      </c>
-      <c r="C350" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
@@ -5350,7 +5350,7 @@
         <v>258</v>
       </c>
       <c r="C351" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -5361,7 +5361,7 @@
         <v>258</v>
       </c>
       <c r="C352" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
@@ -5372,7 +5372,7 @@
         <v>258</v>
       </c>
       <c r="C353" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -5380,10 +5380,10 @@
         <v>0</v>
       </c>
       <c r="B354" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C354" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -5394,7 +5394,7 @@
         <v>257</v>
       </c>
       <c r="C355" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
@@ -5405,7 +5405,7 @@
         <v>257</v>
       </c>
       <c r="C356" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -5416,7 +5416,7 @@
         <v>257</v>
       </c>
       <c r="C357" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
@@ -5424,10 +5424,10 @@
         <v>0</v>
       </c>
       <c r="B358" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C358" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -5438,7 +5438,7 @@
         <v>259</v>
       </c>
       <c r="C359" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
@@ -5449,7 +5449,7 @@
         <v>259</v>
       </c>
       <c r="C360" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
@@ -5460,18 +5460,18 @@
         <v>259</v>
       </c>
       <c r="C361" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>0</v>
-      </c>
-      <c r="B362" t="s">
-        <v>259</v>
-      </c>
-      <c r="C362" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>0</v>
+      </c>
+      <c r="B363" t="s">
+        <v>260</v>
+      </c>
+      <c r="C363" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -5482,7 +5482,7 @@
         <v>260</v>
       </c>
       <c r="C364" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
@@ -5490,10 +5490,10 @@
         <v>0</v>
       </c>
       <c r="B365" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C365" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -5504,7 +5504,7 @@
         <v>263</v>
       </c>
       <c r="C366" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
@@ -5515,7 +5515,7 @@
         <v>263</v>
       </c>
       <c r="C367" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -5523,10 +5523,10 @@
         <v>0</v>
       </c>
       <c r="B368" t="s">
+        <v>266</v>
+      </c>
+      <c r="C368" t="s">
         <v>263</v>
-      </c>
-      <c r="C368" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -5534,10 +5534,10 @@
         <v>0</v>
       </c>
       <c r="B369" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C369" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -5545,10 +5545,10 @@
         <v>0</v>
       </c>
       <c r="B370" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C370" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -5559,7 +5559,7 @@
         <v>264</v>
       </c>
       <c r="C371" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -5570,7 +5570,7 @@
         <v>264</v>
       </c>
       <c r="C372" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -5581,7 +5581,7 @@
         <v>264</v>
       </c>
       <c r="C373" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
@@ -5589,20 +5589,9 @@
         <v>0</v>
       </c>
       <c r="B374" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C374" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A375" t="s">
-        <v>0</v>
-      </c>
-      <c r="B375" t="s">
-        <v>265</v>
-      </c>
-      <c r="C375" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>